<commit_message>
Replaced the IWP 30 Test Data Files.
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/EmulatorData.xlsx
+++ b/KatalonData/IWPTestData/EmulatorData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17239DFE-0960-4324-8F58-34AA25A119F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CC57F7-5E7C-47CB-969A-B2915B84D6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
   </bookViews>
   <sheets>
     <sheet name="PayNowData" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Added NoModifyAmount Test case and data.  Updated Emulator to add Switch Case to handle different MVs.
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/EmulatorData.xlsx
+++ b/KatalonData/IWPTestData/EmulatorData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CC57F7-5E7C-47CB-969A-B2915B84D6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE5DC09-6B12-4FE8-BBB1-AEEF3287484B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
   <si>
     <t>Notes</t>
   </si>
@@ -249,6 +249,12 @@
   </si>
   <si>
     <t>14.50</t>
+  </si>
+  <si>
+    <t>No Modify Amount</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -619,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D3E213-FD08-482B-9ECE-5B5E0D45C129}">
-  <dimension ref="A1:AB5"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,6 +945,86 @@
         <v>31</v>
       </c>
     </row>
+    <row r="6" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
Added Test Case and Data for NoOverPay.
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/EmulatorData.xlsx
+++ b/KatalonData/IWPTestData/EmulatorData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE5DC09-6B12-4FE8-BBB1-AEEF3287484B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058DA352-74C5-4DF0-A359-1606CE1E4951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="75">
   <si>
     <t>Notes</t>
   </si>
@@ -255,6 +255,12 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>26412171</t>
   </si>
 </sst>
 </file>
@@ -625,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D3E213-FD08-482B-9ECE-5B5E0D45C129}">
-  <dimension ref="A1:AB6"/>
+  <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,6 +1031,68 @@
         <v>50</v>
       </c>
     </row>
+    <row r="7" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
Updated Demo Admin Suite Password and other minor updates.
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/EmulatorData.xlsx
+++ b/KatalonData/IWPTestData/EmulatorData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{058DA352-74C5-4DF0-A359-1606CE1E4951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CC1D62-5E55-4987-9CC6-0AD0C76FDDB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
+    <workbookView xWindow="-38510" yWindow="-2030" windowWidth="38620" windowHeight="21220" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
   </bookViews>
   <sheets>
     <sheet name="PayNowData" sheetId="1" r:id="rId1"/>
@@ -637,34 +637,34 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.15234375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.4609375" style="1" customWidth="1"/>
     <col min="3" max="3" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.15234375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.53515625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.69140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.53515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" style="1" customWidth="1"/>
-    <col min="14" max="14" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.53515625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="24" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="16" width="6.15234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.84375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="8.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.3828125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.69140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="8.3046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.15234375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -750,7 +750,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -830,7 +830,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -854,7 +854,7 @@
       </c>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
@@ -931,7 +931,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
@@ -951,7 +951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="29.15" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>71</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="29.15" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
         <v>73</v>
       </c>

</xml_diff>

<commit_message>
Updated Parcel Field Identification.
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/EmulatorData.xlsx
+++ b/KatalonData/IWPTestData/EmulatorData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F692C727-674A-40A4-9023-C65362FE9783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4E7650-A07E-44BE-82C6-485694D29B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="96">
   <si>
     <t>Notes</t>
   </si>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t>26413329</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -831,6 +834,9 @@
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>28</v>
       </c>
@@ -1318,6 +1324,9 @@
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>95</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>81</v>

</xml_diff>

<commit_message>
Updated VRelay25Payments Test Data and Emulator Data.
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/EmulatorData.xlsx
+++ b/KatalonData/IWPTestData/EmulatorData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4E7650-A07E-44BE-82C6-485694D29B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE54F27-8A57-47EC-B65E-9973E35D1A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
+    <workbookView xWindow="1905" yWindow="1545" windowWidth="24840" windowHeight="12570" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
   </bookViews>
   <sheets>
     <sheet name="EmulatorData" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="100">
   <si>
     <t>Notes</t>
   </si>
@@ -324,6 +324,18 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>No Emulator Data</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>26413414</t>
+  </si>
+  <si>
+    <t>Some Company</t>
   </si>
 </sst>
 </file>
@@ -694,17 +706,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D3E213-FD08-482B-9ECE-5B5E0D45C129}">
-  <dimension ref="A1:AF10"/>
+  <dimension ref="A1:AF11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="AB11" sqref="AB11:AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
@@ -719,7 +731,7 @@
     <col min="15" max="15" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" style="1" customWidth="1"/>
     <col min="19" max="19" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="20" max="25" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1287,6 +1299,9 @@
       <c r="P9" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="R9" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="S9" s="2" t="s">
         <v>40</v>
       </c>
@@ -1325,9 +1340,6 @@
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="C10" s="1" t="s">
         <v>81</v>
       </c>
@@ -1405,6 +1417,42 @@
       </c>
       <c r="AF10" s="1" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="W11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added IWP25 Test Cases
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/EmulatorData.xlsx
+++ b/KatalonData/IWPTestData/EmulatorData.xlsx
@@ -5,38 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE54F27-8A57-47EC-B65E-9973E35D1A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D74D71-167D-4714-80AC-4870189BFB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1545" windowWidth="24840" windowHeight="12570" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
   </bookViews>
   <sheets>
     <sheet name="EmulatorData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="102">
   <si>
     <t>Notes</t>
   </si>
@@ -336,6 +325,12 @@
   </si>
   <si>
     <t>Some Company</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>No UnderPay</t>
   </si>
 </sst>
 </file>
@@ -706,45 +701,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D3E213-FD08-482B-9ECE-5B5E0D45C129}">
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AF12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB11" sqref="AB11:AC11"/>
+      <selection activeCell="A13" sqref="A13:AC13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" style="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1796875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.81640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.7265625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.42578125" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="1"/>
+    <col min="31" max="31" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.453125" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -842,7 +837,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -925,7 +920,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -949,7 +944,7 @@
       </c>
       <c r="S3" s="2"/>
     </row>
-    <row r="4" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
@@ -1026,7 +1021,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
@@ -1046,7 +1041,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>71</v>
       </c>
@@ -1126,7 +1121,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="C7" s="1" t="s">
         <v>73</v>
       </c>
@@ -1188,7 +1183,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
@@ -1253,7 +1248,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -1336,7 +1331,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -1419,7 +1414,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
@@ -1453,6 +1448,60 @@
       </c>
       <c r="AC11" s="1" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S12" s="2"/>
+      <c r="T12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deferred Test Cases done
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/EmulatorData.xlsx
+++ b/KatalonData/IWPTestData/EmulatorData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D74D71-167D-4714-80AC-4870189BFB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83046C1-A7CB-49EC-B760-31C719B12FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="103">
   <si>
     <t>Notes</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>No UnderPay</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
@@ -701,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D3E213-FD08-482B-9ECE-5B5E0D45C129}">
-  <dimension ref="A1:AF12"/>
+  <dimension ref="A1:AF13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:AC13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1504,6 +1507,39 @@
         <v>42</v>
       </c>
     </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S13" s="2"/>
+      <c r="W13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
Autopay Test cases done
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/EmulatorData.xlsx
+++ b/KatalonData/IWPTestData/EmulatorData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83046C1-A7CB-49EC-B760-31C719B12FBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AFDB9A-9927-4EF8-A150-57DC24F6DAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
   </bookViews>
   <sheets>
     <sheet name="EmulatorData" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="104">
   <si>
     <t>Notes</t>
   </si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
   </si>
 </sst>
 </file>
@@ -704,45 +707,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D3E213-FD08-482B-9ECE-5B5E0D45C129}">
-  <dimension ref="A1:AF13"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AH14" sqref="AH14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1796875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1796875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.81640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.7265625" style="1" customWidth="1"/>
-    <col min="19" max="19" width="23.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="7.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.77734375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="23.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16.453125" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.1796875" style="1"/>
+    <col min="31" max="31" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.44140625" style="1" customWidth="1"/>
+    <col min="33" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -840,7 +843,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>51</v>
       </c>
@@ -923,7 +926,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>52</v>
       </c>
@@ -947,7 +950,7 @@
       </c>
       <c r="S3" s="2"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
@@ -1024,7 +1027,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>59</v>
       </c>
@@ -1044,7 +1047,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>71</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>73</v>
       </c>
@@ -1186,7 +1189,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
@@ -1251,7 +1254,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>51</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -1417,7 +1420,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>96</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>101</v>
       </c>
@@ -1507,7 +1510,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>96</v>
       </c>
@@ -1537,6 +1540,38 @@
         <v>49</v>
       </c>
       <c r="AC13" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC14" s="1" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added rows of data for 3.0 in excel sheet
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/EmulatorData.xlsx
+++ b/KatalonData/IWPTestData/EmulatorData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AFDB9A-9927-4EF8-A150-57DC24F6DAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4748DD3C-4CE2-408F-989A-0E5D191D10D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
   </bookViews>
   <sheets>
     <sheet name="EmulatorData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="107">
   <si>
     <t>Notes</t>
   </si>
@@ -337,6 +337,15 @@
   </si>
   <si>
     <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
   </si>
 </sst>
 </file>
@@ -707,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D3E213-FD08-482B-9ECE-5B5E0D45C129}">
-  <dimension ref="A1:AF14"/>
+  <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AH14" sqref="AH14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1575,6 +1584,179 @@
         <v>50</v>
       </c>
     </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S15" s="2"/>
+      <c r="W15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC15" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="S17" s="2"/>
+      <c r="T17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>

<commit_message>
Description added for test cases, 3.0 rows of data added, smoke test suite created
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/EmulatorData.xlsx
+++ b/KatalonData/IWPTestData/EmulatorData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4748DD3C-4CE2-408F-989A-0E5D191D10D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B1F6A3-F81B-4C14-B271-EFBD5E180FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B75285DF-1640-4994-93D2-6C318038763B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="109">
   <si>
     <t>Notes</t>
   </si>
@@ -346,6 +346,12 @@
   </si>
   <si>
     <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
 </sst>
 </file>
@@ -716,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D3E213-FD08-482B-9ECE-5B5E0D45C129}">
-  <dimension ref="A1:AF17"/>
+  <dimension ref="A1:AF19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1703,7 +1709,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>101</v>
       </c>
@@ -1755,6 +1761,70 @@
       </c>
       <c r="U17" s="1" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC18" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC19" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>